<commit_message>
VI: Modification in Employee Module
</commit_message>
<xml_diff>
--- a/RetentionTool/RetentionTool/Uploads/Book1.xlsx
+++ b/RetentionTool/RetentionTool/Uploads/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vijetha\ImageStore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Projects\ResourceRetentionTool\RetentionTool\RetentionTool\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Employee ID</t>
   </si>
@@ -75,18 +75,12 @@
   </si>
   <si>
     <t>Image</t>
-  </si>
-  <si>
-    <t>Chan</t>
   </si>
   <si>
     <t>Payroll Specialist
 Team Lead, Payroll Operations</t>
   </si>
   <si>
-    <t>21008</t>
-  </si>
-  <si>
     <t>563202007</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>HR</t>
   </si>
   <si>
-    <t>Spiegel</t>
-  </si>
-  <si>
     <t>570221907</t>
   </si>
   <si>
@@ -117,12 +108,6 @@
     <t>Development</t>
   </si>
   <si>
-    <t>Moore</t>
-  </si>
-  <si>
-    <t>21007</t>
-  </si>
-  <si>
     <t>568110707</t>
   </si>
   <si>
@@ -135,13 +120,22 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>ImageTest</t>
-  </si>
-  <si>
-    <t>Test2</t>
+    <t>Abc</t>
+  </si>
+  <si>
+    <t>Pqy</t>
+  </si>
+  <si>
+    <t>rtfg</t>
+  </si>
+  <si>
+    <t>ghygy</t>
+  </si>
+  <si>
+    <t>jhgj</t>
+  </si>
+  <si>
+    <t>nbhj</t>
   </si>
 </sst>
 </file>
@@ -262,15 +256,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>99062</xdr:colOff>
+      <xdr:colOff>129542</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>632460</xdr:colOff>
+      <xdr:colOff>662940</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>670560</xdr:rowOff>
+      <xdr:rowOff>777240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -293,7 +287,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9852662" y="716280"/>
+          <a:off x="9883142" y="822960"/>
           <a:ext cx="533398" cy="624840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -306,13 +300,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>160021</xdr:colOff>
+      <xdr:colOff>91441</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>83821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>906780</xdr:colOff>
+      <xdr:colOff>838200</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>566979</xdr:rowOff>
     </xdr:to>
@@ -337,52 +331,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9913621" y="2766061"/>
+          <a:off x="9845041" y="2766061"/>
           <a:ext cx="746759" cy="483158"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>251317</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>868681</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>479971</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10004917" y="2194560"/>
-          <a:ext cx="617364" cy="419011"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -659,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,104 +673,104 @@
     </row>
     <row r="2" spans="1:17" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>5009</v>
+        <v>5015</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>19</v>
+      <c r="G2" s="5">
+        <v>5012</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L2" s="6">
         <v>18</v>
       </c>
       <c r="M2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>5010</v>
+        <v>5016</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="G3" s="5">
+        <v>5011</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L3" s="6">
         <v>18</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>5011</v>
+        <v>5017</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="G4" s="5">
+        <v>5012</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="L4" s="6">
         <v>18</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>